<commit_message>
Seuil de rentabilité non linéaire - partie 2
</commit_message>
<xml_diff>
--- a/01. Recherche opérationnelle (Operations research - Management science)/02. Non linéaire/00. SEUIL DE RENTABILITE N.L(EVEN BREAKPOINT)/Formule du seuil de rentabilité n.l.xlsx
+++ b/01. Recherche opérationnelle (Operations research - Management science)/02. Non linéaire/00. SEUIL DE RENTABILITE N.L(EVEN BREAKPOINT)/Formule du seuil de rentabilité n.l.xlsx
@@ -278,13 +278,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>185057</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>59871</xdr:rowOff>
+      <xdr:rowOff>59870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>119743</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>59871</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -293,8 +293,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2177143" y="59871"/>
-          <a:ext cx="4201886" cy="4893129"/>
+          <a:off x="2177143" y="59870"/>
+          <a:ext cx="4201886" cy="7799616"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -536,6 +536,112 @@
             <a:tabLst/>
             <a:defRPr/>
           </a:pPr>
+          <a:endParaRPr lang="fr-FR" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" baseline="0"/>
+            <a:t>Si on substitue cette formule décrivant le volume dans la formule du profit, on obtient une formule non linéaire, avec un carré , comme montré dans la copie d'écran à droite, si on la représente en mode graphique, on obtient une courbe continue , avec un maximum ou la pente est égale à 0, ce maximum représente le seuil de rentabilité non linéaire. Le pente = à zéro est la ou la dérivée de la courbe est = à 0 car la dérivée est une mesure de la pente de la courbe.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" baseline="0"/>
+            <a:t>Pour le calculer, il faut calculer la dérivée , puis trouver la valeur pour le plus haut point ou la pente est = à zéro :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="fr-FR"/>
         </a:p>
         <a:p>
@@ -545,44 +651,31 @@
           <a:endParaRPr lang="fr-FR"/>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="fr-FR">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Formule</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> du seuil de rentabilité non linéaire : </a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-FR">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="fr-FR" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" b="1"/>
         </a:p>
         <a:p>
           <a:r>
@@ -700,6 +793,143 @@
         <a:xfrm>
           <a:off x="6395357" y="631372"/>
           <a:ext cx="3476625" cy="3114675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>119742</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>103414</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6449786" y="3831771"/>
+          <a:ext cx="3015343" cy="1333500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>119742</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>385082</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>55789</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6449786" y="3831771"/>
+          <a:ext cx="6638925" cy="6010275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>527958</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38098</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>140433</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3129644" y="5774869"/>
+          <a:ext cx="2050875" cy="2062845"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1000,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>